<commit_message>
Fix age of Andy Nicholls
</commit_message>
<xml_diff>
--- a/data/2020-06-16/SCW Weekly Comp 2020-06-16 (Responses).xlsx
+++ b/data/2020-06-16/SCW Weekly Comp 2020-06-16 (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-06-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8D6E87-114D-41DD-A08C-A74C61B4124B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020F8FBB-CF15-424B-A328-E2265EB385E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1515,9 +1515,9 @@
   </sheetPr>
   <dimension ref="A1:CY118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN55" sqref="AN55"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1527,7 +1527,7 @@
     <col min="7" max="109" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>43998.582043414353</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>19.03</v>
       </c>
     </row>
-    <row r="3" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>43998.585593796292</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>8.1199999999999992</v>
       </c>
     </row>
-    <row r="4" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>43998.590599884265</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>43998.595952951393</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>49.44</v>
       </c>
     </row>
-    <row r="6" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>43998.628187557872</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>43998.633437569442</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>24.12</v>
       </c>
     </row>
-    <row r="8" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>43998.710005185188</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="9" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43998.711137071761</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="10" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>43998.714821122689</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="11" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43998.716571643519</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>14.06</v>
       </c>
     </row>
-    <row r="12" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>43998.718535451393</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>23.99</v>
       </c>
     </row>
-    <row r="13" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>43998.728734571763</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>43998.799923148152</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>43999.669791828703</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="16" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>43999.689027986111</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>43999.692815567134</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>43999.754600775464</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>43999.756815567132</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>20.010000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>43999.75773597222</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>43999.780673333335</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>43999.782161990741</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>43999.959637384258</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>44000.453846701392</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>9.41</v>
       </c>
     </row>
-    <row r="25" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>44000.457924525464</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>44000.461594270833</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>10.46</v>
       </c>
     </row>
-    <row r="27" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>44000.489836273147</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>22.41</v>
       </c>
     </row>
-    <row r="28" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>44000.571192789357</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>44000.579519374995</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>44000.590718587962</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>19.850000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>44000.5984659838</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>12.64</v>
       </c>
     </row>
-    <row r="32" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>44000.607911145838</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>34.92</v>
       </c>
     </row>
-    <row r="33" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>44000.675088368051</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>26.34</v>
       </c>
     </row>
-    <row r="34" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>44000.796446469903</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>44000.839462141201</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>59.02</v>
       </c>
     </row>
-    <row r="36" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>44000.840426423616</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>44000.841155173606</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>44001.003834143514</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>44001.550208854169</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>44001.700096215282</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>56.18</v>
       </c>
     </row>
-    <row r="41" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44001.766308599537</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>44001.77641175926</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>44001.790162256948</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="44" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>44001.79113518518</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>16.260000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44001.795962418983</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>44001.81498998843</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>50.55</v>
       </c>
     </row>
-    <row r="47" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>44001.815766168977</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>17.07</v>
       </c>
     </row>
-    <row r="48" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44001.830465219908</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>40.56</v>
       </c>
     </row>
-    <row r="49" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>44001.831301678241</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="50" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>44001.832072986115</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>40.56</v>
       </c>
     </row>
-    <row r="51" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>44001.880469571755</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>44001.886231145836</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>44001.89194050926</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>44001.925050648148</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>44001.926274849538</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>44001.928068148147</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>44001.929829583329</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>44001.931159675922</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>44002.160699108797</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>26.98</v>
       </c>
     </row>
-    <row r="60" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>44002.482189351853</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:88" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>44002.482883634264</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>18.53</v>
       </c>
     </row>
-    <row r="62" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>44002.675692453704</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>43.87</v>
       </c>
     </row>
-    <row r="63" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>44002.708437002315</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="64" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>44002.709284143522</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>37.07</v>
       </c>
     </row>
-    <row r="65" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>44002.709999155093</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>15.82</v>
       </c>
     </row>
-    <row r="66" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>44002.711264062498</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>44002.712043657404</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="68" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>44002.713505520835</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>14.52</v>
       </c>
     </row>
-    <row r="69" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>44002.714238912042</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>17.149999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>44002.761654525464</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>12.28</v>
       </c>
     </row>
-    <row r="71" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>44002.763098020834</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>43.21</v>
       </c>
     </row>
-    <row r="72" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>44002.7728890625</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>35.869999999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>44002.797607569446</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>44002.804017777773</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>19.54</v>
       </c>
     </row>
-    <row r="75" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>44002.805632511576</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="76" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>44002.806894328707</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>28.27</v>
       </c>
     </row>
-    <row r="77" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>44002.809290462959</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>44002.810281076388</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>44002.848779108797</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="80" spans="1:98" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:98" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>44002.849678472223</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>44002.850537303239</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>44002.859305925929</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="83" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>44002.862230300925</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="84" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>44003.0627303125</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>44003.3533665625</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>26.31</v>
       </c>
     </row>
-    <row r="86" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>44003.620525902777</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>44003.752450740736</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>27.77</v>
       </c>
     </row>
-    <row r="88" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>44003.762465312495</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="89" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>44003.763407615741</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>33.08</v>
       </c>
     </row>
-    <row r="90" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>44003.763694791662</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>166</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>167</v>
@@ -5352,7 +5352,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>44003.764640740745</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>20.62</v>
       </c>
     </row>
-    <row r="92" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>44003.765560462962</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>24.83</v>
       </c>
     </row>
-    <row r="93" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>44003.826356574078</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="94" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>44003.828816400463</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="95" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:103" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>44003.842037372684</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:103" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:103" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>44004.314417800924</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="97" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>44004.320835856481</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>44004.381272789353</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>44004.599651261575</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>44004.681482037035</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="101" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>44004.69246622685</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="102" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>44004.696971238431</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>44004.698343009259</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>24.88</v>
       </c>
     </row>
-    <row r="104" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>44004.722024062503</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>44004.734386226854</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="106" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>44004.87488304398</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="107" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>44004.876177071761</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>17.22</v>
       </c>
     </row>
-    <row r="108" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>44004.894682708335</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>30.12</v>
       </c>
     </row>
-    <row r="109" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>44004.902516180555</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>32.28</v>
       </c>
     </row>
-    <row r="110" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>44004.920291504633</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="111" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>44004.922730763894</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>29.96</v>
       </c>
     </row>
-    <row r="112" spans="1:93" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:93" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>44005.165376643519</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="113" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>44005.166560740741</v>
       </c>
@@ -6235,7 +6235,7 @@
         <v>28.24</v>
       </c>
     </row>
-    <row r="114" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>44005.168444675925</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>44005.169507847226</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="116" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>44005.170540983796</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>29.69</v>
       </c>
     </row>
-    <row r="117" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>44005.264779050922</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>20.54</v>
       </c>
     </row>
-    <row r="118" spans="1:88" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:88" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>44005.322182118056</v>
       </c>
@@ -6424,9 +6424,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:DE118" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
+    <filterColumn colId="1">
       <filters>
-        <filter val="6x6x6"/>
+        <filter val="Andy Nicholls"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>